<commit_message>
Update data files - Bot run at 2026-02-12 05:02:12 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -534,16 +534,16 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0008333333333333334</v>
+        <v>0.0009027777777777777</v>
       </c>
       <c r="K2" t="n">
-        <v>3213</v>
+        <v>3690</v>
       </c>
       <c r="L2" t="n">
-        <v>0.006426</v>
+        <v>0.00738</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-12 10:15:34 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -534,16 +534,16 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0009722222222222222</v>
+        <v>0.001041666666666667</v>
       </c>
       <c r="K2" t="n">
-        <v>4157</v>
+        <v>4400</v>
       </c>
       <c r="L2" t="n">
-        <v>0.008314</v>
+        <v>0.008800000000000001</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
@@ -636,16 +636,16 @@
         <v>500000</v>
       </c>
       <c r="I4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J4" t="n">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="K4" t="n">
-        <v>71</v>
+        <v>540</v>
       </c>
       <c r="L4" t="n">
-        <v>0.000142</v>
+        <v>0.00108</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>
@@ -1146,16 +1146,16 @@
         <v>500000</v>
       </c>
       <c r="I14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J14" t="n">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="K14" t="n">
-        <v>48</v>
+        <v>290</v>
       </c>
       <c r="L14" t="n">
-        <v>9.6e-05</v>
+        <v>0.00058</v>
       </c>
       <c r="M14" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-12 10:27:45 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -687,16 +687,16 @@
         <v>500000</v>
       </c>
       <c r="I5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J5" t="n">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="K5" t="n">
-        <v>77</v>
+        <v>634</v>
       </c>
       <c r="L5" t="n">
-        <v>0.000154</v>
+        <v>0.001268</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
@@ -942,16 +942,16 @@
         <v>300000</v>
       </c>
       <c r="I10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J10" t="n">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="K10" t="n">
-        <v>51</v>
+        <v>609</v>
       </c>
       <c r="L10" t="n">
-        <v>0.00017</v>
+        <v>0.00203</v>
       </c>
       <c r="M10" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-12 16:16:18 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -534,20 +534,20 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>0.001180555555555556</v>
+        <v>6.944444444444444e-05</v>
       </c>
       <c r="K2" t="n">
-        <v>5381</v>
+        <v>472</v>
       </c>
       <c r="L2" t="n">
-        <v>0.010762</v>
+        <v>0.000944</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>2026-02-11T13:27:13.091680</t>
+          <t>2026-02-12T16:16:10.958439</t>
         </is>
       </c>
     </row>
@@ -585,20 +585,20 @@
         <v>100000</v>
       </c>
       <c r="I3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>712</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>0.00712</v>
+        <v>0</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>2026-02-11T13:27:13.091680</t>
+          <t>2026-02-12T16:16:10.958439</t>
         </is>
       </c>
     </row>
@@ -636,20 +636,20 @@
         <v>500000</v>
       </c>
       <c r="I4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>540</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>0.00108</v>
+        <v>0</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>2026-02-11T13:27:13.091680</t>
+          <t>2026-02-12T16:16:10.958439</t>
         </is>
       </c>
     </row>
@@ -687,20 +687,20 @@
         <v>500000</v>
       </c>
       <c r="I5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>634</v>
+        <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>0.001268</v>
+        <v>0</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>2026-02-11T13:27:13.091680</t>
+          <t>2026-02-12T16:16:10.958439</t>
         </is>
       </c>
     </row>
@@ -738,20 +738,20 @@
         <v>500000</v>
       </c>
       <c r="I6" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>0.0004861111111111111</v>
+        <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>826</v>
+        <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>0.001652</v>
+        <v>0</v>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>2026-02-11T13:27:13.091680</t>
+          <t>2026-02-12T16:16:10.958439</t>
         </is>
       </c>
     </row>
@@ -789,20 +789,20 @@
         <v>500000</v>
       </c>
       <c r="I7" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>0.0004166666666666667</v>
+        <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>983</v>
+        <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>0.001966</v>
+        <v>0</v>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>2026-02-11T13:27:13.091680</t>
+          <t>2026-02-12T16:16:10.958439</t>
         </is>
       </c>
     </row>
@@ -840,20 +840,20 @@
         <v>500000</v>
       </c>
       <c r="I8" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>0.0004166666666666667</v>
+        <v>0</v>
       </c>
       <c r="K8" t="n">
-        <v>590</v>
+        <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>0.00118</v>
+        <v>0</v>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>2026-02-11T13:27:13.091680</t>
+          <t>2026-02-12T16:16:10.958439</t>
         </is>
       </c>
     </row>
@@ -891,20 +891,20 @@
         <v>300000</v>
       </c>
       <c r="I9" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>307</v>
+        <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>0.001023333333333333</v>
+        <v>0</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>2026-02-11T13:27:13.091680</t>
+          <t>2026-02-12T16:16:10.958439</t>
         </is>
       </c>
     </row>
@@ -942,20 +942,20 @@
         <v>300000</v>
       </c>
       <c r="I10" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>609</v>
+        <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>0.00203</v>
+        <v>0</v>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>2026-02-11T13:27:13.091680</t>
+          <t>2026-02-12T16:16:10.958439</t>
         </is>
       </c>
     </row>
@@ -993,20 +993,20 @@
         <v>200000</v>
       </c>
       <c r="I11" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>286</v>
+        <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>0.00143</v>
+        <v>0</v>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>2026-02-11T13:27:13.091680</t>
+          <t>2026-02-12T16:16:10.958439</t>
         </is>
       </c>
     </row>
@@ -1044,20 +1044,20 @@
         <v>200000</v>
       </c>
       <c r="I12" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="K12" t="n">
-        <v>519</v>
+        <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>0.002595</v>
+        <v>0</v>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>2026-02-11T13:27:13.091680</t>
+          <t>2026-02-12T16:16:10.958439</t>
         </is>
       </c>
     </row>
@@ -1095,20 +1095,20 @@
         <v>200000</v>
       </c>
       <c r="I13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="K13" t="n">
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="L13" t="n">
-        <v>0.000255</v>
+        <v>0</v>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>2026-02-11T13:27:13.091680</t>
+          <t>2026-02-12T16:16:10.958439</t>
         </is>
       </c>
     </row>
@@ -1146,20 +1146,20 @@
         <v>500000</v>
       </c>
       <c r="I14" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J14" t="n">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="K14" t="n">
-        <v>290</v>
+        <v>0</v>
       </c>
       <c r="L14" t="n">
-        <v>0.00058</v>
+        <v>0</v>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>2026-02-11T13:27:13.091680</t>
+          <t>2026-02-12T16:16:10.958439</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-12 20:40:24 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -687,16 +687,16 @@
         <v>500000</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>713</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>0.001426</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-12 22:38:16 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -942,16 +942,16 @@
         <v>300000</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>532</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>0.001773333333333333</v>
       </c>
       <c r="M10" t="inlineStr">
         <is>
@@ -993,16 +993,16 @@
         <v>200000</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>562</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>0.00281</v>
       </c>
       <c r="M11" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-13 02:42:16 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -1044,16 +1044,16 @@
         <v>200000</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>475</v>
       </c>
       <c r="L12" t="n">
-        <v>0</v>
+        <v>0.002375</v>
       </c>
       <c r="M12" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-13 07:27:57 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -534,16 +534,16 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0001388888888888889</v>
+        <v>0.0002083333333333333</v>
       </c>
       <c r="K2" t="n">
-        <v>937</v>
+        <v>1409</v>
       </c>
       <c r="L2" t="n">
-        <v>0.001874</v>
+        <v>0.002818</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-14 08:01:08 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -534,20 +534,20 @@
         <v>500000</v>
       </c>
       <c r="I2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0002777777777777778</v>
+        <v>6.944444444444444e-05</v>
       </c>
       <c r="K2" t="n">
-        <v>1922</v>
+        <v>238</v>
       </c>
       <c r="L2" t="n">
-        <v>0.003844</v>
+        <v>0.000476</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>2026-02-12T16:16:10.958439</t>
+          <t>2026-02-14T08:00:33.383907</t>
         </is>
       </c>
     </row>
@@ -585,20 +585,20 @@
         <v>100000</v>
       </c>
       <c r="I3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>469</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>0.00469</v>
+        <v>0</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>2026-02-12T16:16:10.958439</t>
+          <t>2026-02-14T08:00:33.383907</t>
         </is>
       </c>
     </row>
@@ -636,20 +636,20 @@
         <v>500000</v>
       </c>
       <c r="I4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>494</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0009879999999999999</v>
+        <v>0</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>2026-02-12T16:16:10.958439</t>
+          <t>2026-02-14T08:00:33.383907</t>
         </is>
       </c>
     </row>
@@ -687,20 +687,20 @@
         <v>500000</v>
       </c>
       <c r="I5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>713</v>
+        <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>0.001426</v>
+        <v>0</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>2026-02-12T16:16:10.958439</t>
+          <t>2026-02-14T08:00:33.383907</t>
         </is>
       </c>
     </row>
@@ -751,7 +751,7 @@
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>2026-02-12T16:16:10.958439</t>
+          <t>2026-02-14T08:00:33.383907</t>
         </is>
       </c>
     </row>
@@ -802,7 +802,7 @@
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>2026-02-12T16:16:10.958439</t>
+          <t>2026-02-14T08:00:33.383907</t>
         </is>
       </c>
     </row>
@@ -853,7 +853,7 @@
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>2026-02-12T16:16:10.958439</t>
+          <t>2026-02-14T08:00:33.383907</t>
         </is>
       </c>
     </row>
@@ -891,20 +891,20 @@
         <v>300000</v>
       </c>
       <c r="I9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>486</v>
+        <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>0.00162</v>
+        <v>0</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>2026-02-12T16:16:10.958439</t>
+          <t>2026-02-14T08:00:33.383907</t>
         </is>
       </c>
     </row>
@@ -942,20 +942,20 @@
         <v>300000</v>
       </c>
       <c r="I10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>532</v>
+        <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>0.001773333333333333</v>
+        <v>0</v>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>2026-02-12T16:16:10.958439</t>
+          <t>2026-02-14T08:00:33.383907</t>
         </is>
       </c>
     </row>
@@ -993,20 +993,20 @@
         <v>200000</v>
       </c>
       <c r="I11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>562</v>
+        <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>0.00281</v>
+        <v>0</v>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>2026-02-12T16:16:10.958439</t>
+          <t>2026-02-14T08:00:33.383907</t>
         </is>
       </c>
     </row>
@@ -1044,20 +1044,20 @@
         <v>200000</v>
       </c>
       <c r="I12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="K12" t="n">
-        <v>475</v>
+        <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>0.002375</v>
+        <v>0</v>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>2026-02-12T16:16:10.958439</t>
+          <t>2026-02-14T08:00:33.383907</t>
         </is>
       </c>
     </row>
@@ -1108,7 +1108,7 @@
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>2026-02-12T16:16:10.958439</t>
+          <t>2026-02-14T08:00:33.383907</t>
         </is>
       </c>
     </row>
@@ -1146,20 +1146,20 @@
         <v>500000</v>
       </c>
       <c r="I14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="K14" t="n">
-        <v>483</v>
+        <v>0</v>
       </c>
       <c r="L14" t="n">
-        <v>0.000966</v>
+        <v>0</v>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>2026-02-12T16:16:10.958439</t>
+          <t>2026-02-14T08:00:33.383907</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-14 17:01:04 UTC
</commit_message>
<xml_diff>
--- a/Free_API_Load_balancer/Limits.xlsx
+++ b/Free_API_Load_balancer/Limits.xlsx
@@ -585,16 +585,16 @@
         <v>100000</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>241</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>0.00241</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>

</xml_diff>